<commit_message>
Update portfolio-changes.xlsx on 2025-08-17 08:02:26
</commit_message>
<xml_diff>
--- a/portfolio-changes.xlsx
+++ b/portfolio-changes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,6 +471,22 @@
         <v>318.3999938964844</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-08-17 08:02:26</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>60.06000137329102</v>
+      </c>
+      <c r="C3" t="n">
+        <v>664.5999755859375</v>
+      </c>
+      <c r="D3" t="n">
+        <v>318.3999938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>